<commit_message>
Adapted ORCA code rotation axis selection
The rotation axis are selected such that one is on the xy plane. This makes it easier to select rotation angles, if there are asymmetric obstacles.
</commit_message>
<xml_diff>
--- a/src/Quadrotor_States1.xlsx
+++ b/src/Quadrotor_States1.xlsx
@@ -428,784 +428,784 @@
     </row>
     <row r="2" spans="1:7">
       <c r="A2">
-        <v>220.00058521165266</v>
+        <v>220.00026959066784</v>
       </c>
       <c r="B2">
-        <v>250.00168013729635</v>
+        <v>250.00072582102888</v>
       </c>
       <c r="C2">
-        <v>10.864939153266704</v>
+        <v>10.864927139321171</v>
       </c>
       <c r="D2">
-        <v>0.9999991636641616</v>
+        <v>0.9999997243416573</v>
       </c>
       <c r="E2">
-        <v>-0.002410300915191863</v>
+        <v>-0.0010412608900588801</v>
       </c>
       <c r="F2">
-        <v>0.0008395365263134299</v>
+        <v>0.0003867540448786701</v>
       </c>
       <c r="G2">
-        <v>1.6083605012322702e-9</v>
+        <v>-1.0487571689399101e-16</v>
       </c>
     </row>
     <row r="3" spans="1:7">
       <c r="A3">
-        <v>219.98571921366795</v>
+        <v>219.99273067256067</v>
       </c>
       <c r="B3">
-        <v>249.9967983683734</v>
+        <v>250.00143886042096</v>
       </c>
       <c r="C3">
-        <v>11.650163032935579</v>
+        <v>11.65047097814216</v>
       </c>
       <c r="D3">
-        <v>0.9997490203041695</v>
+        <v>0.9999439909785484</v>
       </c>
       <c r="E3">
-        <v>0.007267470319224173</v>
+        <v>-0.0010652922919146992</v>
       </c>
       <c r="F3">
-        <v>-0.022140724594210494</v>
+        <v>-0.01123764832025641</v>
       </c>
       <c r="G3">
-        <v>-0.0003203973995197328</v>
+        <v>-2.6498588398049186e-6</v>
       </c>
     </row>
     <row r="4" spans="1:7">
       <c r="A4">
-        <v>219.96963381621924</v>
+        <v>219.98482525636933</v>
       </c>
       <c r="B4">
-        <v>249.9915358818329</v>
+        <v>250.0021779609179</v>
       </c>
       <c r="C4">
-        <v>12.363614069572765</v>
+        <v>12.363793598199235</v>
       </c>
       <c r="D4">
-        <v>0.9996733061388057</v>
+        <v>0.9999332887766554</v>
       </c>
       <c r="E4">
-        <v>0.008131811155070147</v>
+        <v>-0.001145912195236593</v>
       </c>
       <c r="F4">
-        <v>-0.02484215504191628</v>
+        <v>-0.012221470947576212</v>
       </c>
       <c r="G4">
-        <v>-2.1934756237047996e-5</v>
+        <v>-3.0199053615329836e-6</v>
       </c>
     </row>
     <row r="5" spans="1:7">
       <c r="A5">
-        <v>219.95288703052648</v>
+        <v>219.97664596688688</v>
       </c>
       <c r="B5">
-        <v>249.98605454214774</v>
+        <v>250.002942479048</v>
       </c>
       <c r="C5">
-        <v>13.011381053777908</v>
+        <v>13.011525438739707</v>
       </c>
       <c r="D5">
-        <v>0.999620886009978</v>
+        <v>0.9999231552673236</v>
       </c>
       <c r="E5">
-        <v>0.008765663824147257</v>
+        <v>-0.0012273724887350728</v>
       </c>
       <c r="F5">
-        <v>-0.026763404478887625</v>
+        <v>-0.01308612498073136</v>
       </c>
       <c r="G5">
-        <v>-0.00010692853502706234</v>
+        <v>-2.8583672499424103e-6</v>
       </c>
     </row>
     <row r="6" spans="1:7">
       <c r="A6">
-        <v>219.9354412260046</v>
+        <v>219.96449995234218</v>
       </c>
       <c r="B6">
-        <v>249.98033644764675</v>
+        <v>249.95724406499687</v>
       </c>
       <c r="C6">
-        <v>13.599391420745148</v>
+        <v>13.61950846179564</v>
       </c>
       <c r="D6">
-        <v>0.9995620095884905</v>
+        <v>0.9970140514007063</v>
       </c>
       <c r="E6">
-        <v>0.009443997784961404</v>
+        <v>0.07463022813286826</v>
       </c>
       <c r="F6">
-        <v>-0.02879035049832363</v>
+        <v>-0.019834565490675724</v>
       </c>
       <c r="G6">
-        <v>-0.0003507695769766792</v>
+        <v>1.1050578884936881e-5</v>
       </c>
     </row>
     <row r="7" spans="1:7">
       <c r="A7">
-        <v>219.89016242679884</v>
+        <v>219.92773771811352</v>
       </c>
       <c r="B7">
-        <v>249.9736413246062</v>
+        <v>249.91059641175895</v>
       </c>
       <c r="C7">
-        <v>14.152946838743171</v>
+        <v>14.184271806018279</v>
       </c>
       <c r="D7">
-        <v>0.9970282361004321</v>
+        <v>0.9950620863234991</v>
       </c>
       <c r="E7">
-        <v>0.011267579330743557</v>
+        <v>0.0779421975263948</v>
       </c>
       <c r="F7">
-        <v>-0.07620679113326266</v>
+        <v>-0.06142401491881902</v>
       </c>
       <c r="G7">
-        <v>1.663317614358357e-5</v>
+        <v>2.4695313743101066e-5</v>
       </c>
     </row>
     <row r="8" spans="1:7">
       <c r="A8">
-        <v>219.84317984333694</v>
+        <v>219.88961695483405</v>
       </c>
       <c r="B8">
-        <v>249.9666945109946</v>
+        <v>249.86222542773598</v>
       </c>
       <c r="C8">
-        <v>14.658004671751165</v>
+        <v>14.701036800776686</v>
       </c>
       <c r="D8">
-        <v>0.9966190327979575</v>
+        <v>0.9943953189752971</v>
       </c>
       <c r="E8">
-        <v>0.012016170998704806</v>
+        <v>0.08301959626795787</v>
       </c>
       <c r="F8">
-        <v>-0.08127274325362915</v>
+        <v>-0.06542597445942969</v>
       </c>
       <c r="G8">
-        <v>1.9942948563673247e-5</v>
+        <v>2.7287183986506357e-5</v>
       </c>
     </row>
     <row r="9" spans="1:7">
       <c r="A9">
-        <v>219.79184266001974</v>
+        <v>219.85011030953697</v>
       </c>
       <c r="B9">
-        <v>249.96232251980584</v>
+        <v>249.81209652400972</v>
       </c>
       <c r="C9">
-        <v>15.121479148612895</v>
+        <v>15.174524982587489</v>
       </c>
       <c r="D9">
-        <v>0.9958237261722371</v>
+        <v>0.993671690646245</v>
       </c>
       <c r="E9">
-        <v>0.007744899928202327</v>
+        <v>0.08819537115938278</v>
       </c>
       <c r="F9">
-        <v>-0.0909547551144338</v>
+        <v>-0.06950562808979209</v>
       </c>
       <c r="G9">
-        <v>2.970827758888134e-5</v>
+        <v>3.05186162253215e-5</v>
       </c>
     </row>
     <row r="10" spans="1:7">
       <c r="A10">
-        <v>219.7386565924339</v>
+        <v>219.8091936407595</v>
       </c>
       <c r="B10">
-        <v>249.95779347778824</v>
+        <v>249.76017934668008</v>
       </c>
       <c r="C10">
-        <v>15.545364552430074</v>
+        <v>15.609023440746506</v>
       </c>
       <c r="D10">
-        <v>0.9953006588811085</v>
+        <v>0.9928915770009736</v>
       </c>
       <c r="E10">
-        <v>0.008213401674886317</v>
+        <v>0.09344958080035048</v>
       </c>
       <c r="F10">
-        <v>-0.09646588064581017</v>
+        <v>-0.07364748446434037</v>
       </c>
       <c r="G10">
-        <v>3.524210886130508e-5</v>
+        <v>3.535272598553793e-5</v>
       </c>
     </row>
     <row r="11" spans="1:7">
       <c r="A11">
-        <v>219.68360497225834</v>
+        <v>219.73954619148384</v>
       </c>
       <c r="B11">
-        <v>249.95310603561583</v>
+        <v>249.7093907453672</v>
       </c>
       <c r="C11">
-        <v>15.93349591494203</v>
+        <v>16.036125602006088</v>
       </c>
       <c r="D11">
-        <v>0.9947407424428625</v>
+        <v>0.9878272011837405</v>
       </c>
       <c r="E11">
-        <v>0.00868643448664138</v>
+        <v>0.09159283523281816</v>
       </c>
       <c r="F11">
-        <v>-0.10203225738493932</v>
+        <v>-0.12560094001206648</v>
       </c>
       <c r="G11">
-        <v>4.152475841748826e-5</v>
+        <v>0.00023278098363854814</v>
       </c>
     </row>
     <row r="12" spans="1:7">
       <c r="A12">
-        <v>219.6280352401519</v>
+        <v>219.6679373819163</v>
       </c>
       <c r="B12">
-        <v>249.91513788816243</v>
+        <v>249.65727047873946</v>
       </c>
       <c r="C12">
-        <v>16.30286242372074</v>
+        <v>16.431731619286747</v>
       </c>
       <c r="D12">
-        <v>0.9920198164283532</v>
+        <v>0.9866532613061523</v>
       </c>
       <c r="E12">
-        <v>0.07109969022393654</v>
+        <v>0.09575575674976064</v>
       </c>
       <c r="F12">
-        <v>-0.10406060611631066</v>
+        <v>-0.13155928247910997</v>
       </c>
       <c r="G12">
-        <v>5.047645517739511e-5</v>
+        <v>0.000758463146040114</v>
       </c>
     </row>
     <row r="13" spans="1:7">
       <c r="A13">
-        <v>219.57060380925685</v>
+        <v>219.5936353126526</v>
       </c>
       <c r="B13">
-        <v>249.8758992069551</v>
+        <v>249.6031638789197</v>
       </c>
       <c r="C13">
-        <v>16.6432206113271</v>
+        <v>16.79915182549215</v>
       </c>
       <c r="D13">
-        <v>0.9911606162393027</v>
+        <v>0.9851200694359724</v>
       </c>
       <c r="E13">
-        <v>0.07480725895539334</v>
+        <v>0.10109282957644561</v>
       </c>
       <c r="F13">
-        <v>-0.10949086672347515</v>
+        <v>-0.13882107301457708</v>
       </c>
       <c r="G13">
-        <v>6.223104300065633e-5</v>
+        <v>0.0006753678387950495</v>
       </c>
     </row>
     <row r="14" spans="1:7">
       <c r="A14">
-        <v>219.4358659756421</v>
+        <v>219.51704466106307</v>
       </c>
       <c r="B14">
-        <v>249.84676253675048</v>
+        <v>249.54739052195106</v>
       </c>
       <c r="C14">
-        <v>17.098464082547054</v>
+        <v>17.141267464514595</v>
       </c>
       <c r="D14">
-        <v>0.9698281079707619</v>
+        <v>0.9836858700548914</v>
       </c>
       <c r="E14">
-        <v>0.05121006894347428</v>
+        <v>0.10581198030765823</v>
       </c>
       <c r="F14">
-        <v>-0.2367573279475672</v>
+        <v>-0.14529834759271987</v>
       </c>
       <c r="G14">
-        <v>-0.02136314330467509</v>
+        <v>0.0007052212097034686</v>
       </c>
     </row>
     <row r="15" spans="1:7">
       <c r="A15">
-        <v>219.30194799549744</v>
+        <v>219.43825361630363</v>
       </c>
       <c r="B15">
-        <v>249.80703170513732</v>
+        <v>249.4898368554855</v>
       </c>
       <c r="C15">
-        <v>17.524073738635998</v>
+        <v>17.460648132730213</v>
       </c>
       <c r="D15">
-        <v>0.9677264080384714</v>
+        <v>0.9821956661599742</v>
       </c>
       <c r="E15">
-        <v>0.07100110713045249</v>
+        <v>0.1107167547391844</v>
       </c>
       <c r="F15">
-        <v>-0.23926880494469863</v>
+        <v>-0.15155674076719589</v>
       </c>
       <c r="G15">
-        <v>-0.02947330961447239</v>
+        <v>-0.00010830276304162355</v>
       </c>
     </row>
     <row r="16" spans="1:7">
       <c r="A16">
-        <v>219.16858115125265</v>
+        <v>219.35629592404143</v>
       </c>
       <c r="B16">
-        <v>249.76593618742135</v>
+        <v>249.4298201276793</v>
       </c>
       <c r="C16">
-        <v>17.918739788094165</v>
+        <v>17.76103615358067</v>
       </c>
       <c r="D16">
-        <v>0.9664138274954533</v>
+        <v>0.9802270793194887</v>
       </c>
       <c r="E16">
-        <v>0.07478892558907928</v>
+        <v>0.11678155688779235</v>
       </c>
       <c r="F16">
-        <v>-0.2426607223989864</v>
+        <v>-0.15945745455814336</v>
       </c>
       <c r="G16">
-        <v>-0.03449535362172515</v>
+        <v>-0.0008415078396036129</v>
       </c>
     </row>
     <row r="17" spans="1:7">
       <c r="A17">
-        <v>219.0360471680865</v>
+        <v>219.27155215296693</v>
       </c>
       <c r="B17">
-        <v>249.72652973188298</v>
+        <v>249.36791777525917</v>
       </c>
       <c r="C17">
-        <v>18.282047092519786</v>
+        <v>18.044254614897454</v>
       </c>
       <c r="D17">
-        <v>0.9656322162872768</v>
+        <v>0.978428224325585</v>
       </c>
       <c r="E17">
-        <v>0.07309939215650657</v>
+        <v>0.12171379750330237</v>
       </c>
       <c r="F17">
-        <v>-0.24579845576282983</v>
+        <v>-0.1665963224076738</v>
       </c>
       <c r="G17">
-        <v>-0.03739415708888262</v>
+        <v>-0.0001500672239981155</v>
       </c>
     </row>
     <row r="18" spans="1:7">
       <c r="A18">
-        <v>218.90643276999663</v>
+        <v>219.18373270558683</v>
       </c>
       <c r="B18">
-        <v>249.687016995963</v>
+        <v>249.30378772476186</v>
       </c>
       <c r="C18">
-        <v>18.611117264480463</v>
+        <v>18.313073776788997</v>
       </c>
       <c r="D18">
-        <v>0.9654132451312101</v>
+        <v>0.9764019892059159</v>
       </c>
       <c r="E18">
-        <v>0.07489978544245231</v>
+        <v>0.12718615280986426</v>
       </c>
       <c r="F18">
-        <v>-0.24563980035919356</v>
+        <v>-0.17412788308371938</v>
       </c>
       <c r="G18">
-        <v>-0.04032358381312098</v>
+        <v>-0.000126314245383111</v>
       </c>
     </row>
     <row r="19" spans="1:7">
       <c r="A19">
-        <v>218.77941299740962</v>
+        <v>219.09240583672084</v>
       </c>
       <c r="B19">
-        <v>249.64750437889927</v>
+        <v>249.237084917124</v>
       </c>
       <c r="C19">
-        <v>18.90974196908085</v>
+        <v>18.570781151422633</v>
       </c>
       <c r="D19">
-        <v>0.9652176508171757</v>
+        <v>0.9740983017081197</v>
       </c>
       <c r="E19">
-        <v>0.07638549939943823</v>
+        <v>0.13308863671314408</v>
       </c>
       <c r="F19">
-        <v>-0.24549662801694133</v>
+        <v>-0.18224852323641422</v>
       </c>
       <c r="G19">
-        <v>-0.042930754844790364</v>
+        <v>-0.00020590113756349736</v>
       </c>
     </row>
     <row r="20" spans="1:7">
       <c r="A20">
-        <v>218.65471538288625</v>
+        <v>218.99805314206876</v>
       </c>
       <c r="B20">
-        <v>249.60824860478368</v>
+        <v>249.16816036031378</v>
       </c>
       <c r="C20">
-        <v>19.180951270711137</v>
+        <v>18.818419429590847</v>
       </c>
       <c r="D20">
-        <v>0.965087993592333</v>
+        <v>0.9719910328905776</v>
       </c>
       <c r="E20">
-        <v>0.07727184751781993</v>
+        <v>0.13830638275267207</v>
       </c>
       <c r="F20">
-        <v>-0.2453990441650445</v>
+        <v>-0.18937242504301446</v>
       </c>
       <c r="G20">
-        <v>-0.04473098367944417</v>
+        <v>-0.0002832467056612076</v>
       </c>
     </row>
     <row r="21" spans="1:7">
       <c r="A21">
-        <v>218.53209677724968</v>
+        <v>218.9004431336227</v>
       </c>
       <c r="B21">
-        <v>249.5694688390706</v>
+        <v>249.09684267918848</v>
       </c>
       <c r="C21">
-        <v>19.427461059376064</v>
+        <v>19.058398769305143</v>
       </c>
       <c r="D21">
-        <v>0.9650202022383452</v>
+        <v>0.9697294460284326</v>
       </c>
       <c r="E21">
-        <v>0.07761152312917609</v>
+        <v>0.14368148135113584</v>
       </c>
       <c r="F21">
-        <v>-0.2453424351470296</v>
+        <v>-0.19670736604813496</v>
       </c>
       <c r="G21">
-        <v>-0.04587509458039295</v>
+        <v>-0.0003824864448885051</v>
       </c>
     </row>
     <row r="22" spans="1:7">
       <c r="A22">
-        <v>218.41133598560455</v>
+        <v>218.7991381217443</v>
       </c>
       <c r="B22">
-        <v>249.5313179260719</v>
+        <v>249.02282470289032</v>
       </c>
       <c r="C22">
-        <v>19.65175048321527</v>
+        <v>19.29367728205434</v>
       </c>
       <c r="D22">
-        <v>0.9650065977975348</v>
+        <v>0.9672127206048771</v>
       </c>
       <c r="E22">
-        <v>0.07752173583156224</v>
+        <v>0.1494309480434845</v>
       </c>
       <c r="F22">
-        <v>-0.2453231384134756</v>
+        <v>-0.20454993919117218</v>
       </c>
       <c r="G22">
-        <v>-0.04640571238072501</v>
+        <v>-0.0004253820547333859</v>
       </c>
     </row>
     <row r="23" spans="1:7">
       <c r="A23">
-        <v>218.29354473536694</v>
+        <v>218.6940412213525</v>
       </c>
       <c r="B23">
-        <v>249.49371140766607</v>
+        <v>248.94602157809973</v>
       </c>
       <c r="C23">
-        <v>19.840888379593554</v>
+        <v>19.526499669690068</v>
       </c>
       <c r="D23">
-        <v>0.9648603576284541</v>
+        <v>0.9646205428510412</v>
       </c>
       <c r="E23">
-        <v>0.0783056251392049</v>
+        <v>0.1551065403605994</v>
       </c>
       <c r="F23">
-        <v>-0.24520763320371572</v>
+        <v>-0.21228604447546987</v>
       </c>
       <c r="G23">
-        <v>-0.04863360020689205</v>
+        <v>-0.0005439700505425281</v>
       </c>
     </row>
     <row r="24" spans="1:7">
       <c r="A24">
-        <v>218.18195298531137</v>
+        <v>218.5834715295162</v>
       </c>
       <c r="B24">
-        <v>249.45586428063535</v>
+        <v>248.86343590137713</v>
       </c>
       <c r="C24">
-        <v>19.957808876694184</v>
+        <v>19.764696659492888</v>
       </c>
       <c r="D24">
-        <v>0.9640922563094885</v>
+        <v>0.9605501480147939</v>
       </c>
       <c r="E24">
-        <v>0.0830009720217959</v>
+        <v>0.16585870930781635</v>
       </c>
       <c r="F24">
-        <v>-0.24466233620902675</v>
+        <v>-0.2220583877815519</v>
       </c>
       <c r="G24">
-        <v>-0.0577165021709476</v>
+        <v>-0.00437740028453201</v>
       </c>
     </row>
     <row r="25" spans="1:7">
       <c r="A25">
-        <v>218.07949514286761</v>
+        <v>218.47715381161638</v>
       </c>
       <c r="B25">
-        <v>249.42694456435726</v>
+        <v>248.78292683252894</v>
       </c>
       <c r="C25">
-        <v>19.999999998503363</v>
+        <v>19.938735321279754</v>
       </c>
       <c r="D25">
-        <v>0.9679302417517675</v>
+        <v>0.9597028230279327</v>
       </c>
       <c r="E25">
-        <v>0.06730956742683408</v>
+        <v>0.1690233745090312</v>
       </c>
       <c r="F25">
-        <v>-0.2383993947490234</v>
+        <v>-0.2232051291347308</v>
       </c>
       <c r="G25">
-        <v>-0.037422052315263646</v>
+        <v>-0.007367470239883023</v>
       </c>
     </row>
     <row r="26" spans="1:7">
       <c r="A26">
-        <v>217.9814201416911</v>
+        <v>218.37177475810373</v>
       </c>
       <c r="B26">
-        <v>249.4016104649938</v>
+        <v>248.75622717838903</v>
       </c>
       <c r="C26">
-        <v>19.999999999581252</v>
+        <v>19.99999999936089</v>
       </c>
       <c r="D26">
-        <v>0.9691809088482969</v>
+        <v>0.9670473932501742</v>
       </c>
       <c r="E26">
-        <v>0.06103515984944297</v>
+        <v>0.0611917894232326</v>
       </c>
       <c r="F26">
-        <v>-0.23622176379672713</v>
+        <v>-0.24142079628490096</v>
       </c>
       <c r="G26">
-        <v>-0.029089802462847283</v>
+        <v>-0.04918256278121028</v>
       </c>
     </row>
     <row r="27" spans="1:7">
       <c r="A27">
-        <v>217.88334419254628</v>
+        <v>218.27369679799597</v>
       </c>
       <c r="B27">
-        <v>249.3764331734895</v>
+        <v>248.7370425735193</v>
       </c>
       <c r="C27">
-        <v>19.999999999479822</v>
+        <v>19.99999999948656</v>
       </c>
       <c r="D27">
-        <v>0.9692030429895556</v>
+        <v>0.9700268010717867</v>
       </c>
       <c r="E27">
-        <v>0.06065817223281178</v>
+        <v>0.04624375911219666</v>
       </c>
       <c r="F27">
-        <v>-0.23622666195856007</v>
+        <v>-0.23633359705444645</v>
       </c>
       <c r="G27">
-        <v>-0.029108624847759598</v>
+        <v>-0.02751738408388585</v>
       </c>
     </row>
     <row r="28" spans="1:7">
       <c r="A28">
-        <v>217.7852673131237</v>
+        <v>218.17561967543168</v>
       </c>
       <c r="B28">
-        <v>249.35141670685692</v>
+        <v>248.71801138394537</v>
       </c>
       <c r="C28">
-        <v>19.999999999552255</v>
+        <v>19.999999999480522</v>
       </c>
       <c r="D28">
-        <v>0.9692257148013458</v>
+        <v>0.970047135924364</v>
       </c>
       <c r="E28">
-        <v>0.06027151750673952</v>
+        <v>0.045874550605186235</v>
       </c>
       <c r="F28">
-        <v>-0.23623158794703897</v>
+        <v>-0.23633421033063828</v>
       </c>
       <c r="G28">
-        <v>-0.029124626293885167</v>
+        <v>-0.027420979976970277</v>
       </c>
     </row>
     <row r="29" spans="1:7">
       <c r="A29">
-        <v>217.6881568024326</v>
+        <v>218.0775434490379</v>
       </c>
       <c r="B29">
-        <v>249.3102662406494</v>
+        <v>248.69913643830455</v>
       </c>
       <c r="C29">
-        <v>19.999973338914785</v>
+        <v>19.999999999456506</v>
       </c>
       <c r="D29">
-        <v>0.9669803953382589</v>
+        <v>0.9700677931555529</v>
       </c>
       <c r="E29">
-        <v>0.09902275697937851</v>
+        <v>0.04549852424099319</v>
       </c>
       <c r="F29">
-        <v>-0.23366719066906652</v>
+        <v>-0.23633472903153888</v>
       </c>
       <c r="G29">
-        <v>-0.01366272394383405</v>
+        <v>-0.027320095940505197</v>
       </c>
     </row>
     <row r="30" spans="1:7">
       <c r="A30">
-        <v>217.59017212748435</v>
+        <v>217.97946817994898</v>
       </c>
       <c r="B30">
-        <v>249.27392953243205</v>
+        <v>248.6804206497972</v>
       </c>
       <c r="C30">
-        <v>19.999999999999996</v>
+        <v>19.999999999479446</v>
       </c>
       <c r="D30">
-        <v>0.9674805635895125</v>
+        <v>0.9700887795180559</v>
       </c>
       <c r="E30">
-        <v>0.08745962349261129</v>
+        <v>0.04511547591503826</v>
       </c>
       <c r="F30">
-        <v>-0.2358153304194267</v>
+        <v>-0.2363351483561987</v>
       </c>
       <c r="G30">
-        <v>-0.019380304816140257</v>
+        <v>-0.027214541252565897</v>
       </c>
     </row>
     <row r="31" spans="1:7">
       <c r="A31">
-        <v>217.49218884942448</v>
+        <v>217.8813939317542</v>
       </c>
       <c r="B31">
-        <v>249.23766203360248</v>
+        <v>248.66186701948467</v>
       </c>
       <c r="C31">
-        <v>19.999999999503782</v>
+        <v>19.999999999485386</v>
       </c>
       <c r="D31">
-        <v>0.967493119650474</v>
+        <v>0.9701101018036861</v>
       </c>
       <c r="E31">
-        <v>0.08729474877401346</v>
+        <v>0.04472519349626339</v>
       </c>
       <c r="F31">
-        <v>-0.2358163617464908</v>
+        <v>-0.2363354633750834</v>
       </c>
       <c r="G31">
-        <v>-0.01948997305334382</v>
+        <v>-0.027104115938104342</v>
       </c>
     </row>
     <row r="32" spans="1:7">
       <c r="A32">
-        <v>217.39420548553323</v>
+        <v>217.78332077065375</v>
       </c>
       <c r="B32">
-        <v>249.20146427271652</v>
+        <v>248.643478639795</v>
       </c>
       <c r="C32">
-        <v>19.99999999951916</v>
+        <v>19.99999999948542</v>
       </c>
       <c r="D32">
-        <v>0.9675056356860117</v>
+        <v>0.9701317668554412</v>
       </c>
       <c r="E32">
-        <v>0.08712746358031456</v>
+        <v>0.04432745640182336</v>
       </c>
       <c r="F32">
-        <v>-0.23581789065142766</v>
+        <v>-0.23633566893326208</v>
       </c>
       <c r="G32">
-        <v>-0.01960427349104179</v>
+        <v>-0.026988610219126102</v>
       </c>
     </row>
     <row r="33" spans="1:7">
       <c r="A33">
-        <v>217.29622201630602</v>
+        <v>217.6852487655373</v>
       </c>
       <c r="B33">
-        <v>249.1653380764468</v>
+        <v>248.62525869817247</v>
       </c>
       <c r="C33">
-        <v>19.999999999545704</v>
+        <v>19.999999999547505</v>
       </c>
       <c r="D33">
-        <v>0.9675184413990688</v>
+        <v>0.9701537815408353</v>
       </c>
       <c r="E33">
-        <v>0.08695579278233265</v>
+        <v>0.04392203521981299</v>
       </c>
       <c r="F33">
-        <v>-0.23581949690650686</v>
+        <v>-0.23633575968294565</v>
       </c>
       <c r="G33">
-        <v>-0.019720816820295115</v>
+        <v>-0.026867803988810612</v>
       </c>
     </row>
     <row r="34" spans="1:7">
       <c r="A34">
-        <v>217.1982384210091</v>
+        <v>217.58717798805597</v>
       </c>
       <c r="B34">
-        <v>249.1292853532004</v>
+        <v>248.60721048089178</v>
       </c>
       <c r="C34">
-        <v>19.999999999538023</v>
+        <v>19.999999999576055</v>
       </c>
       <c r="D34">
-        <v>0.9675315488096282</v>
+        <v>0.9701761527308134</v>
       </c>
       <c r="E34">
-        <v>0.08677954003438632</v>
+        <v>0.04350869130727064</v>
       </c>
       <c r="F34">
-        <v>-0.2358211847257291</v>
+        <v>-0.2363357300837116</v>
       </c>
       <c r="G34">
-        <v>-0.01983967704252755</v>
+        <v>-0.026741466261453677</v>
       </c>
     </row>
     <row r="35" spans="1:7">
       <c r="A35">
-        <v>217.10025467757475</v>
+        <v>217.48910851268698</v>
       </c>
       <c r="B35">
-        <v>249.09330809827745</v>
+        <v>248.5893373770382</v>
       </c>
       <c r="C35">
-        <v>19.999999999561123</v>
+        <v>19.999999999546677</v>
       </c>
       <c r="D35">
-        <v>0.9675449706482163</v>
+        <v>0.9701988872744668</v>
       </c>
       <c r="E35">
-        <v>0.08659849658240687</v>
+        <v>0.043087176385877425</v>
       </c>
       <c r="F35">
-        <v>-0.23582295861989902</v>
+        <v>-0.23633557440215588</v>
       </c>
       <c r="G35">
-        <v>-0.019960931760626816</v>
+        <v>-0.02660935461909175</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added Data Analysis Script and Implemented Granular Variables
</commit_message>
<xml_diff>
--- a/src/Quadrotor_States1.xlsx
+++ b/src/Quadrotor_States1.xlsx
@@ -397,7 +397,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CAF0E20E-E4D8-9B45-9C94-E89B574F109C}">
-  <dimension ref="A1:G11"/>
+  <dimension ref="A1:G41"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -428,232 +428,922 @@
     </row>
     <row r="2" spans="1:7">
       <c r="A2">
-        <v>2.4373547650235228</v>
+        <v>221.18100781869654</v>
       </c>
       <c r="B2">
-        <v>10.000171692043867</v>
+        <v>248.65027019548796</v>
       </c>
       <c r="C2">
-        <v>5.046896471093081</v>
+        <v>12.039667294867701</v>
       </c>
       <c r="D2">
-        <v>0.999981022809138</v>
+        <v>0.9999821987688595</v>
       </c>
       <c r="E2">
-        <v>-4.61724764650336e-6</v>
+        <v>-0.0046957997055400115</v>
       </c>
       <c r="F2">
-        <v>-0.004121139566539029</v>
+        <v>-0.004109959780787532</v>
       </c>
       <c r="G2">
-        <v>-5.916092827724651e-5</v>
+        <v>-6.459956137019816e-6</v>
       </c>
     </row>
     <row r="3" spans="1:7">
       <c r="A3">
-        <v>1.361676085171322</v>
+        <v>220.56627883954286</v>
       </c>
       <c r="B3">
-        <v>10.00010278874458</v>
+        <v>248.4221160237972</v>
       </c>
       <c r="C3">
-        <v>4.938313116563589</v>
+        <v>15.221164094879283</v>
       </c>
       <c r="D3">
-        <v>0.9999344451486989</v>
+        <v>1.0000001741968176</v>
       </c>
       <c r="E3">
-        <v>-7.869582588977063e-6</v>
+        <v>-0.00020847873022889586</v>
       </c>
       <c r="F3">
-        <v>0.004596647444976041</v>
+        <v>0.00019580075581956084</v>
       </c>
       <c r="G3">
-        <v>-0.0006704303452623146</v>
+        <v>-0.00035032889254501995</v>
       </c>
     </row>
     <row r="4" spans="1:7">
       <c r="A4">
-        <v>2.983795637694331</v>
+        <v>220.03405821460885</v>
       </c>
       <c r="B4">
-        <v>10.000064397258233</v>
+        <v>247.9123435744799</v>
       </c>
       <c r="C4">
-        <v>4.892919134351777</v>
+        <v>18.50571128918559</v>
       </c>
       <c r="D4">
-        <v>0.9999518369853281</v>
+        <v>1.0000033203192293</v>
       </c>
       <c r="E4">
-        <v>-8.466208017113327e-6</v>
+        <v>0.00017696352110831116</v>
       </c>
       <c r="F4">
-        <v>-0.0038461606004198527</v>
+        <v>-3.4329814445032943e-6</v>
       </c>
       <c r="G4">
-        <v>0.004784530913786008</v>
+        <v>-0.0008825267206975216</v>
       </c>
     </row>
     <row r="5" spans="1:7">
       <c r="A5">
-        <v>2.784998815719126</v>
+        <v>219.158609641191</v>
       </c>
       <c r="B5">
-        <v>10.000030051428933</v>
+        <v>246.5363563736462</v>
       </c>
       <c r="C5">
-        <v>4.877197570609773</v>
+        <v>21.212148296490977</v>
       </c>
       <c r="D5">
-        <v>0.9999645225733925</v>
+        <v>0.9999852070974644</v>
       </c>
       <c r="E5">
-        <v>6.895571787073774e-7</v>
+        <v>-0.004818574756352868</v>
       </c>
       <c r="F5">
-        <v>0.0026473161015748144</v>
+        <v>0.0030648987186341634</v>
       </c>
       <c r="G5">
-        <v>0.000564001257041785</v>
+        <v>-5.325466486794458e-6</v>
       </c>
     </row>
     <row r="6" spans="1:7">
       <c r="A6">
-        <v>3.7317568857085277</v>
+        <v>218.05963608776602</v>
       </c>
       <c r="B6">
-        <v>10.000033594190894</v>
+        <v>244.83465891796195</v>
       </c>
       <c r="C6">
-        <v>4.877947009849106</v>
+        <v>23.351492491895407</v>
       </c>
       <c r="D6">
-        <v>0.9999680883885863</v>
+        <v>0.9999774264370134</v>
       </c>
       <c r="E6">
-        <v>-8.661172426643459e-7</v>
+        <v>-0.005853593644597631</v>
       </c>
       <c r="F6">
-        <v>-0.0016373293783903946</v>
+        <v>0.0037788051782304067</v>
       </c>
       <c r="G6">
-        <v>0.00045499391459529045</v>
+        <v>-1.1704471310455561e-5</v>
       </c>
     </row>
     <row r="7" spans="1:7">
       <c r="A7">
-        <v>3.981453875245893</v>
+        <v>217.8736744925583</v>
       </c>
       <c r="B7">
-        <v>10.000036796395099</v>
+        <v>242.58241086844006</v>
       </c>
       <c r="C7">
-        <v>4.877472886707587</v>
+        <v>24.95715684440649</v>
       </c>
       <c r="D7">
-        <v>0.9999726108619308</v>
+        <v>0.9999721629146696</v>
       </c>
       <c r="E7">
-        <v>8.20449015544594e-6</v>
+        <v>-0.007676342824692908</v>
       </c>
       <c r="F7">
-        <v>0.00036018966531995626</v>
+        <v>0.0006316688820728805</v>
       </c>
       <c r="G7">
-        <v>0.0036043295135268225</v>
+        <v>-1.9453799856415447e-5</v>
       </c>
     </row>
     <row r="8" spans="1:7">
       <c r="A8">
-        <v>4.628221320381994</v>
+        <v>217.54926104036758</v>
       </c>
       <c r="B8">
-        <v>10.00005434776752</v>
+        <v>240.23084334291983</v>
       </c>
       <c r="C8">
-        <v>4.882057738043404</v>
+        <v>26.167895082112764</v>
       </c>
       <c r="D8">
-        <v>0.9999821713421191</v>
+        <v>0.9999695221011593</v>
       </c>
       <c r="E8">
-        <v>-1.0154402459646177e-6</v>
+        <v>-0.007965002387520218</v>
       </c>
       <c r="F8">
-        <v>-7.090598432591845e-5</v>
+        <v>0.0010962931496124617</v>
       </c>
       <c r="G8">
-        <v>0.00255766378405798</v>
+        <v>-2.5477375148211727e-5</v>
       </c>
     </row>
     <row r="9" spans="1:7">
       <c r="A9">
-        <v>5.045855945658361</v>
+        <v>216.60822994603419</v>
       </c>
       <c r="B9">
-        <v>9.88266630113806</v>
+        <v>237.98723859538464</v>
       </c>
       <c r="C9">
-        <v>4.882812839494935</v>
+        <v>27.076000463313193</v>
       </c>
       <c r="D9">
-        <v>0.9999918609741563</v>
+        <v>0.9999682001032707</v>
       </c>
       <c r="E9">
-        <v>0.0002742949187672818</v>
+        <v>-0.007558497698742151</v>
       </c>
       <c r="F9">
-        <v>-0.0003300011280251687</v>
+        <v>0.00316758710025434</v>
       </c>
       <c r="G9">
-        <v>-0.002609481240030512</v>
+        <v>-2.976918115634932e-5</v>
       </c>
     </row>
     <row r="10" spans="1:7">
       <c r="A10">
-        <v>5.587619739066252</v>
+        <v>215.78640969579837</v>
       </c>
       <c r="B10">
-        <v>9.820072065512</v>
+        <v>235.6711903847398</v>
       </c>
       <c r="C10">
-        <v>4.885934171524463</v>
+        <v>27.80581571514462</v>
       </c>
       <c r="D10">
-        <v>0.9999964679761448</v>
+        <v>0.9999677046385246</v>
       </c>
       <c r="E10">
-        <v>-5.139470733387395e-5</v>
+        <v>-0.007785470884820496</v>
       </c>
       <c r="F10">
-        <v>-0.00035729997560886425</v>
+        <v>0.0027597619598279076</v>
       </c>
       <c r="G10">
-        <v>4.01431987834878e-5</v>
+        <v>-3.2640617250434195e-5</v>
       </c>
     </row>
     <row r="11" spans="1:7">
       <c r="A11">
-        <v>6.056965366931687</v>
+        <v>215.48696814158166</v>
       </c>
       <c r="B11">
-        <v>9.768748916722108</v>
+        <v>233.21215904467826</v>
       </c>
       <c r="C11">
-        <v>4.889696845062832</v>
+        <v>28.327015612194895</v>
       </c>
       <c r="D11">
-        <v>1.0000002861086073</v>
+        <v>0.9999673856714704</v>
       </c>
       <c r="E11">
-        <v>2.788086661779225e-6</v>
+        <v>-0.00825336914252565</v>
       </c>
       <c r="F11">
-        <v>0.00012685546742212836</v>
+        <v>0.0010019006943817143</v>
       </c>
       <c r="G11">
-        <v>-0.0015844183477522666</v>
+        <v>-3.5860270619292714e-5</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7">
+      <c r="A12">
+        <v>215.401899302296</v>
+      </c>
+      <c r="B12">
+        <v>230.73007031663775</v>
+      </c>
+      <c r="C12">
+        <v>28.74162417175883</v>
+      </c>
+      <c r="D12">
+        <v>0.9999673272588404</v>
+      </c>
+      <c r="E12">
+        <v>-0.008324130242070753</v>
+      </c>
+      <c r="F12">
+        <v>0.00028199291570476007</v>
+      </c>
+      <c r="G12">
+        <v>-3.7045865164818884e-5</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7">
+      <c r="A13">
+        <v>214.49123412520464</v>
+      </c>
+      <c r="B13">
+        <v>228.4154864206113</v>
+      </c>
+      <c r="C13">
+        <v>29.046887754497842</v>
+      </c>
+      <c r="D13">
+        <v>0.9999673289564005</v>
+      </c>
+      <c r="E13">
+        <v>-0.007736746820324618</v>
+      </c>
+      <c r="F13">
+        <v>0.0030409579766289795</v>
+      </c>
+      <c r="G13">
+        <v>-3.847983911351788e-5</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7">
+      <c r="A14">
+        <v>213.90544924803575</v>
+      </c>
+      <c r="B14">
+        <v>225.99685220187226</v>
+      </c>
+      <c r="C14">
+        <v>29.27968569260369</v>
+      </c>
+      <c r="D14">
+        <v>0.9999673785127546</v>
+      </c>
+      <c r="E14">
+        <v>-0.008083478551196139</v>
+      </c>
+      <c r="F14">
+        <v>0.0019545950484056197</v>
+      </c>
+      <c r="G14">
+        <v>-3.9902413247283925e-5</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7">
+      <c r="A15">
+        <v>213.23656243139817</v>
+      </c>
+      <c r="B15">
+        <v>223.59969972235376</v>
+      </c>
+      <c r="C15">
+        <v>29.460511897344883</v>
+      </c>
+      <c r="D15">
+        <v>0.9999674301258402</v>
+      </c>
+      <c r="E15">
+        <v>-0.008005012308602321</v>
+      </c>
+      <c r="F15">
+        <v>0.0022304825411821015</v>
+      </c>
+      <c r="G15">
+        <v>-4.050397686880136e-5</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7">
+      <c r="A16">
+        <v>212.49642173288873</v>
+      </c>
+      <c r="B16">
+        <v>221.22387190098473</v>
+      </c>
+      <c r="C16">
+        <v>29.59968557021688</v>
+      </c>
+      <c r="D16">
+        <v>0.9999674829409972</v>
+      </c>
+      <c r="E16">
+        <v>-0.007928435190029514</v>
+      </c>
+      <c r="F16">
+        <v>0.0024667649214886274</v>
+      </c>
+      <c r="G16">
+        <v>-4.093429086318503e-5</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7">
+      <c r="A17">
+        <v>211.75637949651875</v>
+      </c>
+      <c r="B17">
+        <v>218.84834309610176</v>
+      </c>
+      <c r="C17">
+        <v>29.714898453815202</v>
+      </c>
+      <c r="D17">
+        <v>0.9999675183575587</v>
+      </c>
+      <c r="E17">
+        <v>-0.00792515056229455</v>
+      </c>
+      <c r="F17">
+        <v>0.002465713537274207</v>
+      </c>
+      <c r="G17">
+        <v>-4.122812964444866e-5</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7">
+      <c r="A18">
+        <v>211.4433750554119</v>
+      </c>
+      <c r="B18">
+        <v>216.38062181731527</v>
+      </c>
+      <c r="C18">
+        <v>29.79228966192382</v>
+      </c>
+      <c r="D18">
+        <v>0.9999675857096433</v>
+      </c>
+      <c r="E18">
+        <v>-0.00823798823908801</v>
+      </c>
+      <c r="F18">
+        <v>0.0010414980644622093</v>
+      </c>
+      <c r="G18">
+        <v>-4.179211247839215e-5</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7">
+      <c r="A19">
+        <v>211.13043736659114</v>
+      </c>
+      <c r="B19">
+        <v>213.91338574887493</v>
+      </c>
+      <c r="C19">
+        <v>29.850449300031396</v>
+      </c>
+      <c r="D19">
+        <v>0.9999676208018002</v>
+      </c>
+      <c r="E19">
+        <v>-0.008234516050324471</v>
+      </c>
+      <c r="F19">
+        <v>0.0010410303555878828</v>
+      </c>
+      <c r="G19">
+        <v>-4.2021439531737215e-5</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7">
+      <c r="A20">
+        <v>209.2737413362654</v>
+      </c>
+      <c r="B20">
+        <v>212.25973566855444</v>
+      </c>
+      <c r="C20">
+        <v>29.89490852457624</v>
+      </c>
+      <c r="D20">
+        <v>0.9999676327582854</v>
+      </c>
+      <c r="E20">
+        <v>-0.0055014365361857704</v>
+      </c>
+      <c r="F20">
+        <v>0.006173930475461611</v>
+      </c>
+      <c r="G20">
+        <v>-3.56051264172308e-5</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7">
+      <c r="A21">
+        <v>207.80167569082997</v>
+      </c>
+      <c r="B21">
+        <v>210.2564400560944</v>
+      </c>
+      <c r="C21">
+        <v>29.927461624129357</v>
+      </c>
+      <c r="D21">
+        <v>0.9999676612155974</v>
+      </c>
+      <c r="E21">
+        <v>-0.006666164472942231</v>
+      </c>
+      <c r="F21">
+        <v>0.004895448641842829</v>
+      </c>
+      <c r="G21">
+        <v>-3.921864217060671e-5</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7">
+      <c r="A22">
+        <v>205.99798208355605</v>
+      </c>
+      <c r="B22">
+        <v>208.54381837127212</v>
+      </c>
+      <c r="C22">
+        <v>29.990260573927387</v>
+      </c>
+      <c r="D22">
+        <v>0.9999677075275305</v>
+      </c>
+      <c r="E22">
+        <v>-0.005698785573334327</v>
+      </c>
+      <c r="F22">
+        <v>0.005998816444858751</v>
+      </c>
+      <c r="G22">
+        <v>-2.998624184389935e-5</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7">
+      <c r="A23">
+        <v>204.47072858508724</v>
+      </c>
+      <c r="B23">
+        <v>206.58448529525197</v>
+      </c>
+      <c r="C23">
+        <v>29.978106033158713</v>
+      </c>
+      <c r="D23">
+        <v>0.9999678198836656</v>
+      </c>
+      <c r="E23">
+        <v>-0.006527559797421635</v>
+      </c>
+      <c r="F23">
+        <v>0.0050850711642669326</v>
+      </c>
+      <c r="G23">
+        <v>-1.7054016713270616e-5</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7">
+      <c r="A24">
+        <v>202.71509660388745</v>
+      </c>
+      <c r="B24">
+        <v>204.80988785097637</v>
+      </c>
+      <c r="C24">
+        <v>29.982723690670404</v>
+      </c>
+      <c r="D24">
+        <v>0.9999707219954665</v>
+      </c>
+      <c r="E24">
+        <v>-0.006220213403067061</v>
+      </c>
+      <c r="F24">
+        <v>0.006137908617136456</v>
+      </c>
+      <c r="G24">
+        <v>0.00020254898035455794</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7">
+      <c r="A25">
+        <v>200.88103271359174</v>
+      </c>
+      <c r="B25">
+        <v>203.1307909872764</v>
+      </c>
+      <c r="C25">
+        <v>29.981269681530513</v>
+      </c>
+      <c r="D25">
+        <v>0.9999728827685518</v>
+      </c>
+      <c r="E25">
+        <v>-0.005304365419305246</v>
+      </c>
+      <c r="F25">
+        <v>0.005789087433497956</v>
+      </c>
+      <c r="G25">
+        <v>2.2146421493649832e-5</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7">
+      <c r="A26">
+        <v>199.23305194508512</v>
+      </c>
+      <c r="B26">
+        <v>201.27453799744492</v>
+      </c>
+      <c r="C26">
+        <v>29.980281416368825</v>
+      </c>
+      <c r="D26">
+        <v>0.99996169076612</v>
+      </c>
+      <c r="E26">
+        <v>-0.006581624665720881</v>
+      </c>
+      <c r="F26">
+        <v>0.005831096131567747</v>
+      </c>
+      <c r="G26">
+        <v>-6.756097592110914e-6</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7">
+      <c r="A27">
+        <v>197.48122701349195</v>
+      </c>
+      <c r="B27">
+        <v>199.51577067840384</v>
+      </c>
+      <c r="C27">
+        <v>29.98005356736122</v>
+      </c>
+      <c r="D27">
+        <v>0.9999617554614583</v>
+      </c>
+      <c r="E27">
+        <v>-0.006235800857297233</v>
+      </c>
+      <c r="F27">
+        <v>0.006198552937839626</v>
+      </c>
+      <c r="G27">
+        <v>-8.631652168844837e-6</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7">
+      <c r="A28">
+        <v>196.20766051146694</v>
+      </c>
+      <c r="B28">
+        <v>197.38534100796343</v>
+      </c>
+      <c r="C28">
+        <v>29.980212747699195</v>
+      </c>
+      <c r="D28">
+        <v>0.9999616784113201</v>
+      </c>
+      <c r="E28">
+        <v>-0.007537010550531586</v>
+      </c>
+      <c r="F28">
+        <v>0.004494774484652369</v>
+      </c>
+      <c r="G28">
+        <v>-7.964280270056797e-6</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7">
+      <c r="A29">
+        <v>195.16336821043046</v>
+      </c>
+      <c r="B29">
+        <v>195.13378830331845</v>
+      </c>
+      <c r="C29">
+        <v>29.98039421928223</v>
+      </c>
+      <c r="D29">
+        <v>0.9999616058130916</v>
+      </c>
+      <c r="E29">
+        <v>-0.00796158844780079</v>
+      </c>
+      <c r="F29">
+        <v>0.0036822459778588805</v>
+      </c>
+      <c r="G29">
+        <v>-7.25895939841492e-6</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7">
+      <c r="A30">
+        <v>194.95974844336286</v>
+      </c>
+      <c r="B30">
+        <v>192.66070326021358</v>
+      </c>
+      <c r="C30">
+        <v>29.97944627497127</v>
+      </c>
+      <c r="D30">
+        <v>0.9999615941906986</v>
+      </c>
+      <c r="E30">
+        <v>-0.008701834901347663</v>
+      </c>
+      <c r="F30">
+        <v>0.0007066032993508339</v>
+      </c>
+      <c r="G30">
+        <v>-1.2995025797603318e-5</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7">
+      <c r="A31">
+        <v>194.26873610881108</v>
+      </c>
+      <c r="B31">
+        <v>190.27706577337335</v>
+      </c>
+      <c r="C31">
+        <v>29.979856573580566</v>
+      </c>
+      <c r="D31">
+        <v>0.9999617378407701</v>
+      </c>
+      <c r="E31">
+        <v>-0.008397538464218939</v>
+      </c>
+      <c r="F31">
+        <v>0.002424348718132206</v>
+      </c>
+      <c r="G31">
+        <v>-1.2499629600942347e-5</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7">
+      <c r="A32">
+        <v>193.50903339614007</v>
+      </c>
+      <c r="B32">
+        <v>187.91442192079367</v>
+      </c>
+      <c r="C32">
+        <v>29.979275872056046</v>
+      </c>
+      <c r="D32">
+        <v>0.9999616706720199</v>
+      </c>
+      <c r="E32">
+        <v>-0.008333944171663669</v>
+      </c>
+      <c r="F32">
+        <v>0.002669637623057387</v>
+      </c>
+      <c r="G32">
+        <v>-1.0550324078800351e-5</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7">
+      <c r="A33">
+        <v>191.87830870731472</v>
+      </c>
+      <c r="B33">
+        <v>186.04285054992192</v>
+      </c>
+      <c r="C33">
+        <v>29.980319189301575</v>
+      </c>
+      <c r="D33">
+        <v>0.9999616758184932</v>
+      </c>
+      <c r="E33">
+        <v>-0.0066362119401152525</v>
+      </c>
+      <c r="F33">
+        <v>0.005770226268265539</v>
+      </c>
+      <c r="G33">
+        <v>-6.817477237873964e-6</v>
+      </c>
+    </row>
+    <row r="34" spans="1:7">
+      <c r="A34">
+        <v>190.0542476837161</v>
+      </c>
+      <c r="B34">
+        <v>184.3590331980119</v>
+      </c>
+      <c r="C34">
+        <v>29.980478112939966</v>
+      </c>
+      <c r="D34">
+        <v>0.9999616850283575</v>
+      </c>
+      <c r="E34">
+        <v>-0.005977948648960714</v>
+      </c>
+      <c r="F34">
+        <v>0.0064627272653590825</v>
+      </c>
+      <c r="G34">
+        <v>-6.532859050504805e-6</v>
+      </c>
+    </row>
+    <row r="35" spans="1:7">
+      <c r="A35">
+        <v>188.07406154432485</v>
+      </c>
+      <c r="B35">
+        <v>182.86179696826505</v>
+      </c>
+      <c r="C35">
+        <v>29.978980880785333</v>
+      </c>
+      <c r="D35">
+        <v>0.9999616871628043</v>
+      </c>
+      <c r="E35">
+        <v>-0.005322190282664798</v>
+      </c>
+      <c r="F35">
+        <v>0.00702434812138624</v>
+      </c>
+      <c r="G35">
+        <v>-6.618834890267468e-6</v>
+      </c>
+    </row>
+    <row r="36" spans="1:7">
+      <c r="A36">
+        <v>186.56511240119116</v>
+      </c>
+      <c r="B36">
+        <v>180.88944699149644</v>
+      </c>
+      <c r="C36">
+        <v>29.98139797030519</v>
+      </c>
+      <c r="D36">
+        <v>0.9999635709946232</v>
+      </c>
+      <c r="E36">
+        <v>-0.006873905702769546</v>
+      </c>
+      <c r="F36">
+        <v>0.005247175796630787</v>
+      </c>
+      <c r="G36">
+        <v>-2.286474532399381e-5</v>
+      </c>
+    </row>
+    <row r="37" spans="1:7">
+      <c r="A37">
+        <v>184.75276576821506</v>
+      </c>
+      <c r="B37">
+        <v>179.19316023047733</v>
+      </c>
+      <c r="C37">
+        <v>29.979641447312115</v>
+      </c>
+      <c r="D37">
+        <v>0.9999616928698494</v>
+      </c>
+      <c r="E37">
+        <v>-0.006021302255941962</v>
+      </c>
+      <c r="F37">
+        <v>0.0064202460968225995</v>
+      </c>
+      <c r="G37">
+        <v>-6.531112963692112e-6</v>
+      </c>
+    </row>
+    <row r="38" spans="1:7">
+      <c r="A38">
+        <v>182.7972742653837</v>
+      </c>
+      <c r="B38">
+        <v>177.66369827593374</v>
+      </c>
+      <c r="C38">
+        <v>29.98086396229764</v>
+      </c>
+      <c r="D38">
+        <v>0.9999616809458268</v>
+      </c>
+      <c r="E38">
+        <v>-0.005435737960208736</v>
+      </c>
+      <c r="F38">
+        <v>0.006935562249265527</v>
+      </c>
+      <c r="G38">
+        <v>-6.578785702334557e-6</v>
+      </c>
+    </row>
+    <row r="39" spans="1:7">
+      <c r="A39">
+        <v>180.66727848783205</v>
+      </c>
+      <c r="B39">
+        <v>176.388279845668</v>
+      </c>
+      <c r="C39">
+        <v>29.98046548483901</v>
+      </c>
+      <c r="D39">
+        <v>0.9999616197024376</v>
+      </c>
+      <c r="E39">
+        <v>-0.004543327990001991</v>
+      </c>
+      <c r="F39">
+        <v>0.007570619902032221</v>
+      </c>
+      <c r="G39">
+        <v>-4.938660464454334e-6</v>
+      </c>
+    </row>
+    <row r="40" spans="1:7">
+      <c r="A40">
+        <v>178.5697719301864</v>
+      </c>
+      <c r="B40">
+        <v>175.060178486701</v>
+      </c>
+      <c r="C40">
+        <v>29.978909703825835</v>
+      </c>
+      <c r="D40">
+        <v>0.9999616878808617</v>
+      </c>
+      <c r="E40">
+        <v>-0.004726058889048028</v>
+      </c>
+      <c r="F40">
+        <v>0.00744772137637659</v>
+      </c>
+      <c r="G40">
+        <v>-6.932433940302185e-6</v>
+      </c>
+    </row>
+    <row r="41" spans="1:7">
+      <c r="A41">
+        <v>176.77066174664006</v>
+      </c>
+      <c r="B41">
+        <v>173.34796754786706</v>
+      </c>
+      <c r="C41">
+        <v>29.98094345042133</v>
+      </c>
+      <c r="D41">
+        <v>0.9999635747867515</v>
+      </c>
+      <c r="E41">
+        <v>-0.005984083751743706</v>
+      </c>
+      <c r="F41">
+        <v>0.006274814216389032</v>
+      </c>
+      <c r="G41">
+        <v>-2.4985686708481202e-5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>